<commit_message>
[items] Minor tweaks to MagAdjust scaling results.
</commit_message>
<xml_diff>
--- a/assets/data/MagAdjust scaling.xlsx
+++ b/assets/data/MagAdjust scaling.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Home\Martin\dev\misc\DarkSoulsCompanion\assets\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\home\martin\dev\misc\DarkSoulsCompanion\assets\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1020" yWindow="0" windowWidth="27780" windowHeight="12420"/>
+    <workbookView xWindow="3060" yWindow="0" windowWidth="27780" windowHeight="12420"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,21 +24,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>Tin Banishment Catalyst scaling</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Intelligence</t>
-  </si>
-  <si>
-    <t>Rounded</t>
   </si>
   <si>
     <t>Actual MagAdjust</t>
   </si>
   <si>
-    <t>Calculated MagAdjust from Rounded</t>
+    <t>Reverse-calculated stat rating</t>
+  </si>
+  <si>
+    <t>Tin Banishment Catalyst scaling:</t>
+  </si>
+  <si>
+    <t>MagAdjust by StatRating</t>
+  </si>
+  <si>
+    <t>StatRating</t>
+  </si>
+  <si>
+    <t>Growth change</t>
   </si>
 </sst>
 </file>
@@ -47,9 +53,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
-    <numFmt numFmtId="169" formatCode="\+0.000"/>
+    <numFmt numFmtId="165" formatCode="\+0.000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -60,6 +66,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -87,14 +100,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -375,69 +389,86 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G93"/>
+  <dimension ref="A1:F93"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.5703125" customWidth="1"/>
     <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="5"/>
+    <col min="3" max="3" width="27.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="22.5703125" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" s="2">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B3" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="D3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C2" s="2">
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>0</v>
-      </c>
-      <c r="B4">
+      <c r="F3" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="3">
         <v>10</v>
       </c>
-      <c r="C4" s="1">
-        <f>((A4 / 100) - 1) / $C$2</f>
-        <v>-0.83333333333333337</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>0</v>
-      </c>
+      <c r="C4" s="4">
+        <f>((A4 / 100) - 1) / $C$1</f>
+        <v>-0.83333333333333337</v>
+      </c>
+      <c r="D4" s="4">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="E4" s="3">
+        <f>100*(1+($C$1*D4))</f>
+        <v>107.80000000000001</v>
+      </c>
+      <c r="F4" s="6">
+        <v>7.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>11</v>
       </c>
       <c r="C5" s="1">
-        <f t="shared" ref="C5:C68" si="0">((A5 / 100) - 1) / $C$2</f>
-        <v>-0.83333333333333337</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <f>((A5 / 100) - 1) / $C$1</f>
+        <v>-0.83333333333333337</v>
+      </c>
+      <c r="D5" s="7">
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="E5">
+        <f>100*(1+($C$1*D5))</f>
+        <v>108.64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>109</v>
       </c>
@@ -445,18 +476,18 @@
         <v>12</v>
       </c>
       <c r="C6" s="1">
-        <f t="shared" si="0"/>
+        <f>((A6 / 100) - 1) / $C$1</f>
         <v>7.5000000000000067E-2</v>
       </c>
       <c r="D6" s="1">
-        <v>7.4999999999999997E-2</v>
+        <v>7.9000000000000001E-2</v>
       </c>
       <c r="E6">
-        <f>100*(1+($C$2*D6))</f>
-        <v>109.00000000000001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <f>100*(1+($C$1*D6))</f>
+        <v>109.48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>110</v>
       </c>
@@ -464,18 +495,18 @@
         <v>13</v>
       </c>
       <c r="C7" s="1">
-        <f t="shared" si="0"/>
+        <f>((A7 / 100) - 1) / $C$1</f>
         <v>8.3333333333333412E-2</v>
       </c>
-      <c r="D7" s="1">
-        <v>8.5000000000000006E-2</v>
+      <c r="D7" s="7">
+        <v>8.5999999999999993E-2</v>
       </c>
       <c r="E7">
-        <f t="shared" ref="E7:E70" si="1">100*(1+($C$2*D7))</f>
-        <v>110.2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <f>100*(1+($C$1*D7))</f>
+        <v>110.32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>111</v>
       </c>
@@ -483,18 +514,18 @@
         <v>14</v>
       </c>
       <c r="C8" s="1">
-        <f t="shared" si="0"/>
+        <f>((A8 / 100) - 1) / $C$1</f>
         <v>9.1666666666666757E-2</v>
       </c>
       <c r="D8" s="1">
-        <v>9.5000000000000001E-2</v>
+        <v>9.2999999999999999E-2</v>
       </c>
       <c r="E8">
-        <f t="shared" si="1"/>
-        <v>111.39999999999999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+        <f>100*(1+($C$1*D8))</f>
+        <v>111.16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>112</v>
       </c>
@@ -502,21 +533,21 @@
         <v>15</v>
       </c>
       <c r="C9" s="4">
-        <f t="shared" si="0"/>
+        <f>((A9 / 100) - 1) / $C$1</f>
         <v>0.10000000000000009</v>
       </c>
       <c r="D9" s="4">
         <v>0.1</v>
       </c>
       <c r="E9" s="3">
-        <f t="shared" si="1"/>
+        <f>100*(1+($C$1*D9))</f>
         <v>112.00000000000001</v>
       </c>
-      <c r="G9" s="6">
+      <c r="F9" s="6">
         <v>0.4</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>116</v>
       </c>
@@ -524,18 +555,18 @@
         <v>16</v>
       </c>
       <c r="C10" s="1">
-        <f t="shared" si="0"/>
+        <f>((A10 / 100) - 1) / $C$1</f>
         <v>0.13333333333333328</v>
       </c>
       <c r="D10" s="1">
         <v>0.14000000000000001</v>
       </c>
       <c r="E10">
-        <f t="shared" si="1"/>
+        <f>100*(1+($C$1*D10))</f>
         <v>116.8</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>121</v>
       </c>
@@ -543,18 +574,18 @@
         <v>17</v>
       </c>
       <c r="C11" s="1">
-        <f t="shared" si="0"/>
+        <f>((A11 / 100) - 1) / $C$1</f>
         <v>0.17499999999999999</v>
       </c>
       <c r="D11" s="1">
         <v>0.18</v>
       </c>
       <c r="E11">
-        <f t="shared" si="1"/>
+        <f>100*(1+($C$1*D11))</f>
         <v>121.6</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>126</v>
       </c>
@@ -562,18 +593,18 @@
         <v>18</v>
       </c>
       <c r="C12" s="1">
-        <f t="shared" si="0"/>
+        <f>((A12 / 100) - 1) / $C$1</f>
         <v>0.21666666666666667</v>
       </c>
       <c r="D12" s="1">
         <v>0.22</v>
       </c>
       <c r="E12">
-        <f t="shared" si="1"/>
+        <f>100*(1+($C$1*D12))</f>
         <v>126.4</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>131</v>
       </c>
@@ -581,18 +612,18 @@
         <v>19</v>
       </c>
       <c r="C13" s="1">
-        <f t="shared" si="0"/>
+        <f>((A13 / 100) - 1) / $C$1</f>
         <v>0.25833333333333341</v>
       </c>
       <c r="D13" s="1">
         <v>0.26</v>
       </c>
       <c r="E13">
-        <f t="shared" si="1"/>
+        <f>100*(1+($C$1*D13))</f>
         <v>131.20000000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>136</v>
       </c>
@@ -600,18 +631,18 @@
         <v>20</v>
       </c>
       <c r="C14" s="1">
-        <f t="shared" si="0"/>
+        <f>((A14 / 100) - 1) / $C$1</f>
         <v>0.3000000000000001</v>
       </c>
       <c r="D14" s="1">
         <v>0.3</v>
       </c>
       <c r="E14">
-        <f t="shared" si="1"/>
+        <f>100*(1+($C$1*D14))</f>
         <v>136</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>140</v>
       </c>
@@ -619,18 +650,18 @@
         <v>21</v>
       </c>
       <c r="C15" s="1">
-        <f t="shared" si="0"/>
+        <f>((A15 / 100) - 1) / $C$1</f>
         <v>0.33333333333333326</v>
       </c>
       <c r="D15" s="1">
         <v>0.34</v>
       </c>
       <c r="E15">
-        <f t="shared" si="1"/>
+        <f>100*(1+($C$1*D15))</f>
         <v>140.79999999999998</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>145</v>
       </c>
@@ -638,151 +669,130 @@
         <v>22</v>
       </c>
       <c r="C16" s="1">
-        <f t="shared" si="0"/>
+        <f>((A16 / 100) - 1) / $C$1</f>
         <v>0.375</v>
       </c>
       <c r="D16" s="1">
         <v>0.38</v>
       </c>
       <c r="E16">
-        <f t="shared" si="1"/>
+        <f>100*(1+($C$1*D16))</f>
         <v>145.6</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>0</v>
-      </c>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>23</v>
       </c>
       <c r="C17" s="1">
-        <f t="shared" si="0"/>
+        <f>((A17 / 100) - 1) / $C$1</f>
         <v>-0.83333333333333337</v>
       </c>
       <c r="D17" s="1">
         <v>0.42</v>
       </c>
       <c r="E17">
-        <f t="shared" si="1"/>
+        <f>100*(1+($C$1*D17))</f>
         <v>150.4</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>0</v>
-      </c>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>24</v>
       </c>
       <c r="C18" s="1">
-        <f t="shared" si="0"/>
+        <f>((A18 / 100) - 1) / $C$1</f>
         <v>-0.83333333333333337</v>
       </c>
       <c r="D18" s="1">
         <v>0.46</v>
       </c>
       <c r="E18">
-        <f t="shared" si="1"/>
+        <f>100*(1+($C$1*D18))</f>
         <v>155.20000000000002</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>0</v>
-      </c>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>25</v>
       </c>
       <c r="C19" s="1">
-        <f t="shared" si="0"/>
+        <f>((A19 / 100) - 1) / $C$1</f>
         <v>-0.83333333333333337</v>
       </c>
       <c r="D19" s="1">
         <v>0.5</v>
       </c>
       <c r="E19">
-        <f t="shared" si="1"/>
+        <f>100*(1+($C$1*D19))</f>
         <v>160</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>0</v>
-      </c>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>26</v>
       </c>
       <c r="C20" s="1">
-        <f t="shared" si="0"/>
+        <f>((A20 / 100) - 1) / $C$1</f>
         <v>-0.83333333333333337</v>
       </c>
       <c r="D20" s="1">
         <v>0.54</v>
       </c>
       <c r="E20">
-        <f t="shared" si="1"/>
+        <f>100*(1+($C$1*D20))</f>
         <v>164.8</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>0</v>
-      </c>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>27</v>
       </c>
       <c r="C21" s="1">
-        <f t="shared" si="0"/>
+        <f>((A21 / 100) - 1) / $C$1</f>
         <v>-0.83333333333333337</v>
       </c>
       <c r="D21" s="1">
         <v>0.57999999999999996</v>
       </c>
       <c r="E21">
-        <f t="shared" si="1"/>
+        <f>100*(1+($C$1*D21))</f>
         <v>169.6</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>0</v>
-      </c>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>28</v>
       </c>
       <c r="C22" s="1">
-        <f t="shared" si="0"/>
+        <f>((A22 / 100) - 1) / $C$1</f>
         <v>-0.83333333333333337</v>
       </c>
       <c r="D22" s="1">
         <v>0.62</v>
       </c>
       <c r="E22">
-        <f t="shared" si="1"/>
+        <f>100*(1+($C$1*D22))</f>
         <v>174.4</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>0</v>
-      </c>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>29</v>
       </c>
       <c r="C23" s="1">
-        <f t="shared" si="0"/>
+        <f>((A23 / 100) - 1) / $C$1</f>
         <v>-0.83333333333333337</v>
       </c>
       <c r="D23" s="1">
         <v>0.66</v>
       </c>
       <c r="E23">
-        <f t="shared" si="1"/>
+        <f>100*(1+($C$1*D23))</f>
         <v>179.20000000000002</v>
       </c>
     </row>
-    <row r="24" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>184</v>
       </c>
@@ -790,21 +800,21 @@
         <v>30</v>
       </c>
       <c r="C24" s="4">
-        <f t="shared" si="0"/>
+        <f>((A24 / 100) - 1) / $C$1</f>
         <v>0.70000000000000007</v>
       </c>
       <c r="D24" s="4">
         <v>0.7</v>
       </c>
       <c r="E24" s="3">
-        <f t="shared" si="1"/>
+        <f>100*(1+($C$1*D24))</f>
         <v>184</v>
       </c>
-      <c r="G24" s="6">
+      <c r="F24" s="6">
         <v>0.01</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>185</v>
       </c>
@@ -812,18 +822,18 @@
         <v>31</v>
       </c>
       <c r="C25" s="1">
-        <f t="shared" si="0"/>
+        <f>((A25 / 100) - 1) / $C$1</f>
         <v>0.70833333333333348</v>
       </c>
       <c r="D25" s="1">
         <v>0.71</v>
       </c>
       <c r="E25">
-        <f t="shared" si="1"/>
+        <f>100*(1+($C$1*D25))</f>
         <v>185.2</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>186</v>
       </c>
@@ -831,56 +841,50 @@
         <v>32</v>
       </c>
       <c r="C26" s="1">
-        <f t="shared" si="0"/>
+        <f>((A26 / 100) - 1) / $C$1</f>
         <v>0.71666666666666679</v>
       </c>
       <c r="D26" s="1">
         <v>0.72</v>
       </c>
       <c r="E26">
-        <f t="shared" si="1"/>
+        <f>100*(1+($C$1*D26))</f>
         <v>186.39999999999998</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>0</v>
-      </c>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B27">
         <v>33</v>
       </c>
       <c r="C27" s="1">
-        <f t="shared" si="0"/>
+        <f>((A27 / 100) - 1) / $C$1</f>
         <v>-0.83333333333333337</v>
       </c>
       <c r="D27" s="1">
         <v>0.73</v>
       </c>
       <c r="E27">
-        <f t="shared" si="1"/>
+        <f>100*(1+($C$1*D27))</f>
         <v>187.6</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>0</v>
-      </c>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B28">
         <v>34</v>
       </c>
       <c r="C28" s="1">
-        <f t="shared" si="0"/>
+        <f>((A28 / 100) - 1) / $C$1</f>
         <v>-0.83333333333333337</v>
       </c>
       <c r="D28" s="1">
         <v>0.74</v>
       </c>
       <c r="E28">
-        <f t="shared" si="1"/>
+        <f>100*(1+($C$1*D28))</f>
         <v>188.79999999999998</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>190</v>
       </c>
@@ -888,94 +892,82 @@
         <v>35</v>
       </c>
       <c r="C29" s="1">
-        <f t="shared" si="0"/>
+        <f>((A29 / 100) - 1) / $C$1</f>
         <v>0.75</v>
       </c>
       <c r="D29" s="1">
         <v>0.75</v>
       </c>
       <c r="E29">
-        <f t="shared" si="1"/>
+        <f>100*(1+($C$1*D29))</f>
         <v>190</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>0</v>
-      </c>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B30">
         <v>36</v>
       </c>
       <c r="C30" s="1">
-        <f t="shared" si="0"/>
+        <f>((A30 / 100) - 1) / $C$1</f>
         <v>-0.83333333333333337</v>
       </c>
       <c r="D30" s="1">
         <v>0.76</v>
       </c>
       <c r="E30">
-        <f t="shared" si="1"/>
+        <f>100*(1+($C$1*D30))</f>
         <v>191.2</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>0</v>
-      </c>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B31">
         <v>37</v>
       </c>
       <c r="C31" s="1">
-        <f t="shared" si="0"/>
+        <f>((A31 / 100) - 1) / $C$1</f>
         <v>-0.83333333333333337</v>
       </c>
       <c r="D31" s="1">
         <v>0.77</v>
       </c>
       <c r="E31">
-        <f t="shared" si="1"/>
+        <f>100*(1+($C$1*D31))</f>
         <v>192.4</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>0</v>
-      </c>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B32">
         <v>38</v>
       </c>
       <c r="C32" s="1">
-        <f t="shared" si="0"/>
+        <f>((A32 / 100) - 1) / $C$1</f>
         <v>-0.83333333333333337</v>
       </c>
       <c r="D32" s="1">
         <v>0.78</v>
       </c>
       <c r="E32">
-        <f t="shared" si="1"/>
+        <f>100*(1+($C$1*D32))</f>
         <v>193.6</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>0</v>
-      </c>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B33">
         <v>39</v>
       </c>
       <c r="C33" s="1">
-        <f t="shared" si="0"/>
+        <f>((A33 / 100) - 1) / $C$1</f>
         <v>-0.83333333333333337</v>
       </c>
       <c r="D33" s="1">
         <v>0.79</v>
       </c>
       <c r="E33">
-        <f t="shared" si="1"/>
+        <f>100*(1+($C$1*D33))</f>
         <v>194.79999999999998</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>196</v>
       </c>
@@ -983,94 +975,82 @@
         <v>40</v>
       </c>
       <c r="C34" s="1">
-        <f t="shared" si="0"/>
+        <f>((A34 / 100) - 1) / $C$1</f>
         <v>0.8</v>
       </c>
       <c r="D34" s="1">
         <v>0.8</v>
       </c>
       <c r="E34">
-        <f t="shared" si="1"/>
+        <f>100*(1+($C$1*D34))</f>
         <v>196</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>0</v>
-      </c>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B35">
         <v>41</v>
       </c>
       <c r="C35" s="1">
-        <f t="shared" si="0"/>
+        <f>((A35 / 100) - 1) / $C$1</f>
         <v>-0.83333333333333337</v>
       </c>
       <c r="D35" s="1">
         <v>0.81</v>
       </c>
       <c r="E35">
-        <f t="shared" si="1"/>
+        <f>100*(1+($C$1*D35))</f>
         <v>197.2</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>0</v>
-      </c>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B36">
         <v>42</v>
       </c>
       <c r="C36" s="1">
-        <f t="shared" si="0"/>
+        <f>((A36 / 100) - 1) / $C$1</f>
         <v>-0.83333333333333337</v>
       </c>
       <c r="D36" s="1">
         <v>0.82</v>
       </c>
       <c r="E36">
-        <f t="shared" si="1"/>
+        <f>100*(1+($C$1*D36))</f>
         <v>198.4</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>0</v>
-      </c>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B37">
         <v>43</v>
       </c>
       <c r="C37" s="1">
-        <f t="shared" si="0"/>
+        <f>((A37 / 100) - 1) / $C$1</f>
         <v>-0.83333333333333337</v>
       </c>
       <c r="D37" s="1">
         <v>0.83</v>
       </c>
       <c r="E37">
-        <f t="shared" si="1"/>
+        <f>100*(1+($C$1*D37))</f>
         <v>199.6</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>0</v>
-      </c>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B38">
         <v>44</v>
       </c>
       <c r="C38" s="1">
-        <f t="shared" si="0"/>
+        <f>((A38 / 100) - 1) / $C$1</f>
         <v>-0.83333333333333337</v>
       </c>
       <c r="D38" s="1">
         <v>0.84</v>
       </c>
       <c r="E38">
-        <f t="shared" si="1"/>
+        <f>100*(1+($C$1*D38))</f>
         <v>200.8</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>202</v>
       </c>
@@ -1078,94 +1058,82 @@
         <v>45</v>
       </c>
       <c r="C39" s="1">
-        <f t="shared" si="0"/>
+        <f>((A39 / 100) - 1) / $C$1</f>
         <v>0.85000000000000009</v>
       </c>
       <c r="D39" s="1">
         <v>0.85</v>
       </c>
       <c r="E39">
-        <f t="shared" si="1"/>
+        <f>100*(1+($C$1*D39))</f>
         <v>202</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>0</v>
-      </c>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B40">
         <v>46</v>
       </c>
       <c r="C40" s="1">
-        <f t="shared" si="0"/>
+        <f>((A40 / 100) - 1) / $C$1</f>
         <v>-0.83333333333333337</v>
       </c>
       <c r="D40" s="1">
         <v>0.86</v>
       </c>
       <c r="E40">
-        <f t="shared" si="1"/>
+        <f>100*(1+($C$1*D40))</f>
         <v>203.2</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>0</v>
-      </c>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B41">
         <v>47</v>
       </c>
       <c r="C41" s="1">
-        <f t="shared" si="0"/>
+        <f>((A41 / 100) - 1) / $C$1</f>
         <v>-0.83333333333333337</v>
       </c>
       <c r="D41" s="1">
         <v>0.87</v>
       </c>
       <c r="E41">
-        <f t="shared" si="1"/>
+        <f>100*(1+($C$1*D41))</f>
         <v>204.4</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>0</v>
-      </c>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B42">
         <v>48</v>
       </c>
       <c r="C42" s="1">
-        <f t="shared" si="0"/>
+        <f>((A42 / 100) - 1) / $C$1</f>
         <v>-0.83333333333333337</v>
       </c>
       <c r="D42" s="1">
         <v>0.88</v>
       </c>
       <c r="E42">
-        <f t="shared" si="1"/>
+        <f>100*(1+($C$1*D42))</f>
         <v>205.6</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <v>0</v>
-      </c>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B43">
         <v>49</v>
       </c>
       <c r="C43" s="1">
-        <f t="shared" si="0"/>
+        <f>((A43 / 100) - 1) / $C$1</f>
         <v>-0.83333333333333337</v>
       </c>
       <c r="D43" s="1">
         <v>0.89</v>
       </c>
       <c r="E43">
-        <f t="shared" si="1"/>
+        <f>100*(1+($C$1*D43))</f>
         <v>206.8</v>
       </c>
     </row>
-    <row r="44" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>208</v>
       </c>
@@ -1173,21 +1141,21 @@
         <v>50</v>
       </c>
       <c r="C44" s="4">
-        <f t="shared" si="0"/>
+        <f>((A44 / 100) - 1) / $C$1</f>
         <v>0.90000000000000013</v>
       </c>
       <c r="D44" s="4">
         <v>0.9</v>
       </c>
       <c r="E44" s="3">
-        <f t="shared" si="1"/>
+        <f>100*(1+($C$1*D44))</f>
         <v>208</v>
       </c>
-      <c r="G44" s="6">
+      <c r="F44" s="6">
         <v>2E-3</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>208</v>
       </c>
@@ -1195,18 +1163,18 @@
         <v>51</v>
       </c>
       <c r="C45" s="1">
-        <f t="shared" si="0"/>
+        <f>((A45 / 100) - 1) / $C$1</f>
         <v>0.90000000000000013</v>
       </c>
       <c r="D45" s="1">
         <v>0.90200000000000002</v>
       </c>
       <c r="E45">
-        <f t="shared" si="1"/>
+        <f>100*(1+($C$1*D45))</f>
         <v>208.23999999999998</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>208</v>
       </c>
@@ -1214,18 +1182,18 @@
         <v>52</v>
       </c>
       <c r="C46" s="1">
-        <f t="shared" si="0"/>
+        <f>((A46 / 100) - 1) / $C$1</f>
         <v>0.90000000000000013</v>
       </c>
       <c r="D46" s="1">
         <v>0.90400000000000003</v>
       </c>
       <c r="E46">
-        <f t="shared" si="1"/>
+        <f>100*(1+($C$1*D46))</f>
         <v>208.48</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>208</v>
       </c>
@@ -1233,18 +1201,18 @@
         <v>53</v>
       </c>
       <c r="C47" s="1">
-        <f t="shared" si="0"/>
+        <f>((A47 / 100) - 1) / $C$1</f>
         <v>0.90000000000000013</v>
       </c>
       <c r="D47" s="1">
         <v>0.90600000000000003</v>
       </c>
       <c r="E47">
-        <f t="shared" si="1"/>
+        <f>100*(1+($C$1*D47))</f>
         <v>208.72000000000003</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>208</v>
       </c>
@@ -1252,14 +1220,14 @@
         <v>54</v>
       </c>
       <c r="C48" s="1">
-        <f t="shared" si="0"/>
+        <f>((A48 / 100) - 1) / $C$1</f>
         <v>0.90000000000000013</v>
       </c>
       <c r="D48" s="1">
         <v>0.90800000000000003</v>
       </c>
       <c r="E48">
-        <f t="shared" si="1"/>
+        <f>100*(1+($C$1*D48))</f>
         <v>208.95999999999998</v>
       </c>
     </row>
@@ -1271,14 +1239,14 @@
         <v>55</v>
       </c>
       <c r="C49" s="1">
-        <f t="shared" si="0"/>
+        <f>((A49 / 100) - 1) / $C$1</f>
         <v>0.90833333333333321</v>
       </c>
       <c r="D49" s="1">
         <v>0.91</v>
       </c>
       <c r="E49">
-        <f t="shared" si="1"/>
+        <f>100*(1+($C$1*D49))</f>
         <v>209.20000000000002</v>
       </c>
     </row>
@@ -1290,14 +1258,14 @@
         <v>56</v>
       </c>
       <c r="C50" s="1">
-        <f t="shared" si="0"/>
+        <f>((A50 / 100) - 1) / $C$1</f>
         <v>0.90833333333333321</v>
       </c>
       <c r="D50" s="1">
         <v>0.91200000000000003</v>
       </c>
       <c r="E50">
-        <f t="shared" si="1"/>
+        <f>100*(1+($C$1*D50))</f>
         <v>209.44000000000003</v>
       </c>
     </row>
@@ -1309,52 +1277,46 @@
         <v>57</v>
       </c>
       <c r="C51" s="1">
-        <f t="shared" si="0"/>
+        <f>((A51 / 100) - 1) / $C$1</f>
         <v>0.90833333333333321</v>
       </c>
       <c r="D51" s="1">
         <v>0.91400000000000003</v>
       </c>
       <c r="E51">
-        <f t="shared" si="1"/>
+        <f>100*(1+($C$1*D51))</f>
         <v>209.68</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52">
-        <v>0</v>
-      </c>
       <c r="B52">
         <v>58</v>
       </c>
       <c r="C52" s="1">
-        <f t="shared" si="0"/>
+        <f>((A52 / 100) - 1) / $C$1</f>
         <v>-0.83333333333333337</v>
       </c>
       <c r="D52" s="1">
         <v>0.91600000000000004</v>
       </c>
       <c r="E52">
-        <f t="shared" si="1"/>
+        <f>100*(1+($C$1*D52))</f>
         <v>209.91999999999996</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53">
-        <v>0</v>
-      </c>
       <c r="B53">
         <v>59</v>
       </c>
       <c r="C53" s="1">
-        <f t="shared" si="0"/>
+        <f>((A53 / 100) - 1) / $C$1</f>
         <v>-0.83333333333333337</v>
       </c>
       <c r="D53" s="1">
         <v>0.91800000000000004</v>
       </c>
       <c r="E53">
-        <f t="shared" si="1"/>
+        <f>100*(1+($C$1*D53))</f>
         <v>210.16</v>
       </c>
     </row>
@@ -1366,90 +1328,78 @@
         <v>60</v>
       </c>
       <c r="C54" s="1">
-        <f t="shared" si="0"/>
+        <f>((A54 / 100) - 1) / $C$1</f>
         <v>0.91666666666666674</v>
       </c>
       <c r="D54" s="1">
         <v>0.92</v>
       </c>
       <c r="E54">
-        <f t="shared" si="1"/>
+        <f>100*(1+($C$1*D54))</f>
         <v>210.4</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55">
-        <v>0</v>
-      </c>
       <c r="B55">
         <v>61</v>
       </c>
       <c r="C55" s="1">
-        <f t="shared" si="0"/>
+        <f>((A55 / 100) - 1) / $C$1</f>
         <v>-0.83333333333333337</v>
       </c>
       <c r="D55" s="1">
         <v>0.92200000000000004</v>
       </c>
       <c r="E55">
-        <f t="shared" si="1"/>
+        <f>100*(1+($C$1*D55))</f>
         <v>210.64</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56">
-        <v>0</v>
-      </c>
       <c r="B56">
         <v>62</v>
       </c>
       <c r="C56" s="1">
-        <f t="shared" si="0"/>
+        <f>((A56 / 100) - 1) / $C$1</f>
         <v>-0.83333333333333337</v>
       </c>
       <c r="D56" s="1">
         <v>0.92400000000000004</v>
       </c>
       <c r="E56">
-        <f t="shared" si="1"/>
+        <f>100*(1+($C$1*D56))</f>
         <v>210.88</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57">
-        <v>0</v>
-      </c>
       <c r="B57">
         <v>63</v>
       </c>
       <c r="C57" s="1">
-        <f t="shared" si="0"/>
+        <f>((A57 / 100) - 1) / $C$1</f>
         <v>-0.83333333333333337</v>
       </c>
       <c r="D57" s="1">
         <v>0.92600000000000005</v>
       </c>
       <c r="E57">
-        <f t="shared" si="1"/>
+        <f>100*(1+($C$1*D57))</f>
         <v>211.12</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58">
-        <v>0</v>
-      </c>
       <c r="B58">
         <v>64</v>
       </c>
       <c r="C58" s="1">
-        <f t="shared" si="0"/>
+        <f>((A58 / 100) - 1) / $C$1</f>
         <v>-0.83333333333333337</v>
       </c>
       <c r="D58" s="1">
         <v>0.92800000000000005</v>
       </c>
       <c r="E58">
-        <f t="shared" si="1"/>
+        <f>100*(1+($C$1*D58))</f>
         <v>211.35999999999999</v>
       </c>
     </row>
@@ -1461,14 +1411,14 @@
         <v>65</v>
       </c>
       <c r="C59" s="1">
-        <f t="shared" si="0"/>
+        <f>((A59 / 100) - 1) / $C$1</f>
         <v>0.92499999999999993</v>
       </c>
       <c r="D59" s="1">
         <v>0.93</v>
       </c>
       <c r="E59">
-        <f t="shared" si="1"/>
+        <f>100*(1+($C$1*D59))</f>
         <v>211.60000000000002</v>
       </c>
     </row>
@@ -1480,14 +1430,14 @@
         <v>66</v>
       </c>
       <c r="C60" s="1">
-        <f t="shared" si="0"/>
+        <f>((A60 / 100) - 1) / $C$1</f>
         <v>0.92499999999999993</v>
       </c>
       <c r="D60" s="1">
         <v>0.93200000000000005</v>
       </c>
       <c r="E60">
-        <f t="shared" si="1"/>
+        <f>100*(1+($C$1*D60))</f>
         <v>211.84000000000003</v>
       </c>
     </row>
@@ -1499,52 +1449,46 @@
         <v>67</v>
       </c>
       <c r="C61" s="1">
-        <f t="shared" si="0"/>
+        <f>((A61 / 100) - 1) / $C$1</f>
         <v>0.93333333333333346</v>
       </c>
       <c r="D61" s="1">
         <v>0.93400000000000005</v>
       </c>
       <c r="E61">
-        <f t="shared" si="1"/>
+        <f>100*(1+($C$1*D61))</f>
         <v>212.08</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62">
-        <v>0</v>
-      </c>
       <c r="B62">
         <v>68</v>
       </c>
       <c r="C62" s="1">
-        <f t="shared" si="0"/>
+        <f>((A62 / 100) - 1) / $C$1</f>
         <v>-0.83333333333333337</v>
       </c>
       <c r="D62" s="1">
         <v>0.93600000000000005</v>
       </c>
       <c r="E62">
-        <f t="shared" si="1"/>
+        <f>100*(1+($C$1*D62))</f>
         <v>212.31999999999996</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63">
-        <v>0</v>
-      </c>
       <c r="B63">
         <v>69</v>
       </c>
       <c r="C63" s="1">
-        <f t="shared" si="0"/>
+        <f>((A63 / 100) - 1) / $C$1</f>
         <v>-0.83333333333333337</v>
       </c>
       <c r="D63" s="1">
         <v>0.93799999999999994</v>
       </c>
       <c r="E63">
-        <f t="shared" si="1"/>
+        <f>100*(1+($C$1*D63))</f>
         <v>212.56</v>
       </c>
     </row>
@@ -1556,18 +1500,18 @@
         <v>70</v>
       </c>
       <c r="C64" s="1">
-        <f t="shared" si="0"/>
+        <f>((A64 / 100) - 1) / $C$1</f>
         <v>0.93333333333333346</v>
       </c>
       <c r="D64" s="1">
         <v>0.94</v>
       </c>
       <c r="E64">
-        <f t="shared" si="1"/>
+        <f>100*(1+($C$1*D64))</f>
         <v>212.8</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>213</v>
       </c>
@@ -1575,75 +1519,66 @@
         <v>71</v>
       </c>
       <c r="C65" s="1">
-        <f t="shared" si="0"/>
+        <f>((A65 / 100) - 1) / $C$1</f>
         <v>0.94166666666666665</v>
       </c>
       <c r="D65" s="1">
         <v>0.94199999999999995</v>
       </c>
       <c r="E65">
-        <f t="shared" si="1"/>
+        <f>100*(1+($C$1*D65))</f>
         <v>213.04</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A66">
-        <v>0</v>
-      </c>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B66">
         <v>72</v>
       </c>
       <c r="C66" s="1">
-        <f t="shared" si="0"/>
+        <f>((A66 / 100) - 1) / $C$1</f>
         <v>-0.83333333333333337</v>
       </c>
       <c r="D66" s="1">
         <v>0.94399999999999995</v>
       </c>
       <c r="E66">
-        <f t="shared" si="1"/>
+        <f>100*(1+($C$1*D66))</f>
         <v>213.27999999999997</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A67">
-        <v>0</v>
-      </c>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B67">
         <v>73</v>
       </c>
       <c r="C67" s="1">
-        <f t="shared" si="0"/>
+        <f>((A67 / 100) - 1) / $C$1</f>
         <v>-0.83333333333333337</v>
       </c>
       <c r="D67" s="1">
         <v>0.94599999999999995</v>
       </c>
       <c r="E67">
-        <f t="shared" si="1"/>
+        <f>100*(1+($C$1*D67))</f>
         <v>213.52</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A68">
-        <v>0</v>
-      </c>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B68">
         <v>74</v>
       </c>
       <c r="C68" s="1">
-        <f t="shared" si="0"/>
+        <f>((A68 / 100) - 1) / $C$1</f>
         <v>-0.83333333333333337</v>
       </c>
       <c r="D68" s="1">
         <v>0.94799999999999995</v>
       </c>
       <c r="E68">
-        <f t="shared" si="1"/>
+        <f>100*(1+($C$1*D68))</f>
         <v>213.76</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>214</v>
       </c>
@@ -1651,94 +1586,82 @@
         <v>75</v>
       </c>
       <c r="C69" s="1">
-        <f t="shared" ref="C69:C93" si="2">((A69 / 100) - 1) / $C$2</f>
+        <f>((A69 / 100) - 1) / $C$1</f>
         <v>0.95000000000000018</v>
       </c>
       <c r="D69" s="1">
         <v>0.95</v>
       </c>
       <c r="E69">
-        <f t="shared" si="1"/>
+        <f>100*(1+($C$1*D69))</f>
         <v>213.99999999999997</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A70">
-        <v>0</v>
-      </c>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B70">
         <v>76</v>
       </c>
       <c r="C70" s="1">
-        <f t="shared" si="2"/>
+        <f>((A70 / 100) - 1) / $C$1</f>
         <v>-0.83333333333333337</v>
       </c>
       <c r="D70" s="1">
         <v>0.95199999999999996</v>
       </c>
       <c r="E70">
-        <f t="shared" si="1"/>
+        <f>100*(1+($C$1*D70))</f>
         <v>214.23999999999998</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A71">
-        <v>0</v>
-      </c>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B71">
         <v>77</v>
       </c>
       <c r="C71" s="1">
-        <f t="shared" si="2"/>
+        <f>((A71 / 100) - 1) / $C$1</f>
         <v>-0.83333333333333337</v>
       </c>
       <c r="D71" s="1">
         <v>0.95399999999999996</v>
       </c>
       <c r="E71">
-        <f t="shared" ref="E71:E93" si="3">100*(1+($C$2*D71))</f>
+        <f>100*(1+($C$1*D71))</f>
         <v>214.48000000000002</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A72">
-        <v>0</v>
-      </c>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B72">
         <v>78</v>
       </c>
       <c r="C72" s="1">
-        <f t="shared" si="2"/>
+        <f>((A72 / 100) - 1) / $C$1</f>
         <v>-0.83333333333333337</v>
       </c>
       <c r="D72" s="1">
         <v>0.95599999999999996</v>
       </c>
       <c r="E72">
-        <f t="shared" si="3"/>
+        <f>100*(1+($C$1*D72))</f>
         <v>214.71999999999997</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A73">
-        <v>0</v>
-      </c>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B73">
         <v>79</v>
       </c>
       <c r="C73" s="1">
-        <f t="shared" si="2"/>
+        <f>((A73 / 100) - 1) / $C$1</f>
         <v>-0.83333333333333337</v>
       </c>
       <c r="D73" s="1">
         <v>0.95799999999999996</v>
       </c>
       <c r="E73">
-        <f t="shared" si="3"/>
+        <f>100*(1+($C$1*D73))</f>
         <v>214.96</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>215</v>
       </c>
@@ -1746,18 +1669,18 @@
         <v>80</v>
       </c>
       <c r="C74" s="1">
-        <f t="shared" si="2"/>
+        <f>((A74 / 100) - 1) / $C$1</f>
         <v>0.95833333333333326</v>
       </c>
       <c r="D74" s="1">
         <v>0.96</v>
       </c>
       <c r="E74">
-        <f t="shared" si="3"/>
+        <f>100*(1+($C$1*D74))</f>
         <v>215.20000000000002</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>215</v>
       </c>
@@ -1765,75 +1688,66 @@
         <v>81</v>
       </c>
       <c r="C75" s="1">
-        <f t="shared" si="2"/>
+        <f>((A75 / 100) - 1) / $C$1</f>
         <v>0.95833333333333326</v>
       </c>
       <c r="D75" s="1">
         <v>0.96199999999999997</v>
       </c>
       <c r="E75">
-        <f t="shared" si="3"/>
+        <f>100*(1+($C$1*D75))</f>
         <v>215.44</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A76">
-        <v>0</v>
-      </c>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B76">
         <v>82</v>
       </c>
       <c r="C76" s="1">
-        <f t="shared" si="2"/>
+        <f>((A76 / 100) - 1) / $C$1</f>
         <v>-0.83333333333333337</v>
       </c>
       <c r="D76" s="1">
         <v>0.96399999999999997</v>
       </c>
       <c r="E76">
-        <f t="shared" si="3"/>
+        <f>100*(1+($C$1*D76))</f>
         <v>215.67999999999995</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A77">
-        <v>0</v>
-      </c>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B77">
         <v>83</v>
       </c>
       <c r="C77" s="1">
-        <f t="shared" si="2"/>
+        <f>((A77 / 100) - 1) / $C$1</f>
         <v>-0.83333333333333337</v>
       </c>
       <c r="D77" s="1">
         <v>0.96599999999999997</v>
       </c>
       <c r="E77">
-        <f t="shared" si="3"/>
+        <f>100*(1+($C$1*D77))</f>
         <v>215.92000000000002</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A78">
-        <v>0</v>
-      </c>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B78">
         <v>84</v>
       </c>
       <c r="C78" s="1">
-        <f t="shared" si="2"/>
+        <f>((A78 / 100) - 1) / $C$1</f>
         <v>-0.83333333333333337</v>
       </c>
       <c r="D78" s="1">
         <v>0.96799999999999997</v>
       </c>
       <c r="E78">
-        <f t="shared" si="3"/>
+        <f>100*(1+($C$1*D78))</f>
         <v>216.16</v>
       </c>
     </row>
-    <row r="79" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="3">
         <v>216</v>
       </c>
@@ -1841,21 +1755,21 @@
         <v>85</v>
       </c>
       <c r="C79" s="4">
-        <f t="shared" si="2"/>
+        <f>((A79 / 100) - 1) / $C$1</f>
         <v>0.96666666666666679</v>
       </c>
       <c r="D79" s="4">
         <v>0.97</v>
       </c>
       <c r="E79" s="3">
-        <f t="shared" si="3"/>
+        <f>100*(1+($C$1*D79))</f>
         <v>216.39999999999998</v>
       </c>
-      <c r="G79" s="6">
+      <c r="F79" s="6">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>216</v>
       </c>
@@ -1863,14 +1777,14 @@
         <v>86</v>
       </c>
       <c r="C80" s="1">
-        <f t="shared" si="2"/>
+        <f>((A80 / 100) - 1) / $C$1</f>
         <v>0.96666666666666679</v>
       </c>
       <c r="D80" s="1">
         <v>0.97250000000000003</v>
       </c>
       <c r="E80">
-        <f t="shared" si="3"/>
+        <f>100*(1+($C$1*D80))</f>
         <v>216.7</v>
       </c>
     </row>
@@ -1882,14 +1796,14 @@
         <v>87</v>
       </c>
       <c r="C81" s="1">
-        <f t="shared" si="2"/>
+        <f>((A81 / 100) - 1) / $C$1</f>
         <v>0.97499999999999998</v>
       </c>
       <c r="D81" s="1">
         <v>0.97499999999999998</v>
       </c>
       <c r="E81">
-        <f t="shared" si="3"/>
+        <f>100*(1+($C$1*D81))</f>
         <v>217</v>
       </c>
     </row>
@@ -1901,14 +1815,14 @@
         <v>88</v>
       </c>
       <c r="C82" s="1">
-        <f t="shared" si="2"/>
+        <f>((A82 / 100) - 1) / $C$1</f>
         <v>0.97499999999999998</v>
       </c>
       <c r="D82" s="1">
         <v>0.97750000000000004</v>
       </c>
       <c r="E82">
-        <f t="shared" si="3"/>
+        <f>100*(1+($C$1*D82))</f>
         <v>217.3</v>
       </c>
     </row>
@@ -1920,14 +1834,14 @@
         <v>89</v>
       </c>
       <c r="C83" s="1">
-        <f t="shared" si="2"/>
+        <f>((A83 / 100) - 1) / $C$1</f>
         <v>0.97499999999999998</v>
       </c>
       <c r="D83" s="1">
         <v>0.98</v>
       </c>
       <c r="E83">
-        <f t="shared" si="3"/>
+        <f>100*(1+($C$1*D83))</f>
         <v>217.60000000000002</v>
       </c>
     </row>
@@ -1939,14 +1853,14 @@
         <v>90</v>
       </c>
       <c r="C84" s="1">
-        <f t="shared" si="2"/>
+        <f>((A84 / 100) - 1) / $C$1</f>
         <v>0.97499999999999998</v>
       </c>
       <c r="D84" s="1">
         <v>0.98250000000000004</v>
       </c>
       <c r="E84">
-        <f t="shared" si="3"/>
+        <f>100*(1+($C$1*D84))</f>
         <v>217.90000000000003</v>
       </c>
     </row>
@@ -1958,14 +1872,14 @@
         <v>91</v>
       </c>
       <c r="C85" s="1">
-        <f t="shared" si="2"/>
+        <f>((A85 / 100) - 1) / $C$1</f>
         <v>0.9833333333333335</v>
       </c>
       <c r="D85" s="1">
         <v>0.98499999999999999</v>
       </c>
       <c r="E85">
-        <f t="shared" si="3"/>
+        <f>100*(1+($C$1*D85))</f>
         <v>218.2</v>
       </c>
     </row>
@@ -1977,14 +1891,14 @@
         <v>92</v>
       </c>
       <c r="C86" s="1">
-        <f t="shared" si="2"/>
+        <f>((A86 / 100) - 1) / $C$1</f>
         <v>0.9833333333333335</v>
       </c>
       <c r="D86" s="1">
         <v>0.98750000000000004</v>
       </c>
       <c r="E86">
-        <f t="shared" si="3"/>
+        <f>100*(1+($C$1*D86))</f>
         <v>218.5</v>
       </c>
     </row>
@@ -1996,14 +1910,14 @@
         <v>93</v>
       </c>
       <c r="C87" s="1">
-        <f t="shared" si="2"/>
+        <f>((A87 / 100) - 1) / $C$1</f>
         <v>0.9833333333333335</v>
       </c>
       <c r="D87" s="1">
         <v>0.99</v>
       </c>
       <c r="E87">
-        <f t="shared" si="3"/>
+        <f>100*(1+($C$1*D87))</f>
         <v>218.79999999999998</v>
       </c>
     </row>
@@ -2015,14 +1929,14 @@
         <v>94</v>
       </c>
       <c r="C88" s="1">
-        <f t="shared" si="2"/>
+        <f>((A88 / 100) - 1) / $C$1</f>
         <v>0.9833333333333335</v>
       </c>
       <c r="D88" s="1">
         <v>0.99250000000000005</v>
       </c>
       <c r="E88">
-        <f t="shared" si="3"/>
+        <f>100*(1+($C$1*D88))</f>
         <v>219.1</v>
       </c>
     </row>
@@ -2034,14 +1948,14 @@
         <v>95</v>
       </c>
       <c r="C89" s="1">
-        <f t="shared" si="2"/>
+        <f>((A89 / 100) - 1) / $C$1</f>
         <v>0.9916666666666667</v>
       </c>
       <c r="D89" s="1">
         <v>0.99500000000000099</v>
       </c>
       <c r="E89">
-        <f t="shared" si="3"/>
+        <f>100*(1+($C$1*D89))</f>
         <v>219.40000000000009</v>
       </c>
     </row>
@@ -2053,14 +1967,14 @@
         <v>96</v>
       </c>
       <c r="C90" s="1">
-        <f t="shared" si="2"/>
+        <f>((A90 / 100) - 1) / $C$1</f>
         <v>0.9916666666666667</v>
       </c>
       <c r="D90" s="1">
         <v>0.99750000000000105</v>
       </c>
       <c r="E90">
-        <f t="shared" si="3"/>
+        <f>100*(1+($C$1*D90))</f>
         <v>219.7000000000001</v>
       </c>
     </row>
@@ -2072,14 +1986,14 @@
         <v>97</v>
       </c>
       <c r="C91" s="1">
-        <f t="shared" si="2"/>
+        <f>((A91 / 100) - 1) / $C$1</f>
         <v>0.9916666666666667</v>
       </c>
       <c r="D91" s="1">
         <v>1</v>
       </c>
       <c r="E91">
-        <f t="shared" si="3"/>
+        <f>100*(1+($C$1*D91))</f>
         <v>220.00000000000003</v>
       </c>
     </row>
@@ -2091,14 +2005,14 @@
         <v>98</v>
       </c>
       <c r="C92" s="1">
-        <f t="shared" si="2"/>
+        <f>((A92 / 100) - 1) / $C$1</f>
         <v>0.9916666666666667</v>
       </c>
       <c r="D92" s="1">
         <v>1.0024999999999999</v>
       </c>
       <c r="E92">
-        <f t="shared" si="3"/>
+        <f>100*(1+($C$1*D92))</f>
         <v>220.29999999999998</v>
       </c>
     </row>
@@ -2110,14 +2024,14 @@
         <v>99</v>
       </c>
       <c r="C93" s="1">
-        <f t="shared" si="2"/>
+        <f>((A93 / 100) - 1) / $C$1</f>
         <v>1.0000000000000002</v>
       </c>
       <c r="D93" s="1">
         <v>1.0049999999999999</v>
       </c>
       <c r="E93">
-        <f t="shared" si="3"/>
+        <f>100*(1+($C$1*D93))</f>
         <v>220.59999999999997</v>
       </c>
     </row>

</xml_diff>